<commit_message>
save 15 12 2025
</commit_message>
<xml_diff>
--- a/4 четверть_9_JavaScript_Vue 3.xlsx
+++ b/4 четверть_9_JavaScript_Vue 3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Machenike\Desktop\GB_Developer_Workbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E996ACE-0E7B-449B-9B57-C807ACC0C933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF03E18-17C2-4D2D-9C4A-A43CD58FFF92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Урок 1 часть 1</t>
   </si>
@@ -68,6 +68,9 @@
       <t xml:space="preserve"> Зайти в браузер - интсрументы разработчика и в консоли написать Vue. Если браузер вернет объект VUE, значит подключен
 </t>
     </r>
+  </si>
+  <si>
+    <t>02 10 00</t>
   </si>
 </sst>
 </file>
@@ -130,7 +133,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -161,6 +164,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -175,7 +184,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -210,6 +219,9 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -547,7 +559,7 @@
   <dimension ref="A2:V17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -633,6 +645,9 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C6" s="9"/>
+      <c r="D6" s="13" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C7" s="9"/>

</xml_diff>

<commit_message>
save 20 01 2026
</commit_message>
<xml_diff>
--- a/4 четверть_9_JavaScript_Vue 3.xlsx
+++ b/4 четверть_9_JavaScript_Vue 3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Machenike\Desktop\GB_Developer_Workbook\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlexServHW\Desktop\GB_Developer_Workbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8CF8C92-2B6A-4017-B66E-DECD80505FA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE60BE8-B58D-4B39-A6E5-BC8D550376E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="База" sheetId="12" r:id="rId1"/>
@@ -22,12 +22,15 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="273">
   <si>
     <t>Урок 1 часть 1</t>
   </si>
@@ -139,13 +142,7 @@
 2 36 00 - key</t>
   </si>
   <si>
-    <t>Разные модификаторы событий</t>
-  </si>
-  <si>
     <t>02 43 00 - https://vuejs.org/guide/essentials/event-handling.html</t>
-  </si>
-  <si>
-    <t>Вызов нескольких функций</t>
   </si>
   <si>
     <t>02 54 00</t>
@@ -4061,9 +4058,6 @@
     <t>a @click.stop.prevent="doThat"&gt;&lt;/a&gt;</t>
   </si>
   <si>
-    <t>.stop.prevent</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -4622,17 +4616,826 @@
       <t xml:space="preserve"> Полезно, когда мы не хотим, чтобы браузер дожидался окончания вызова обработчика, чтобы выполнить заложенную в него логику</t>
     </r>
   </si>
+  <si>
+    <t>Модификаторы клавиш</t>
+  </si>
+  <si>
+    <t>`https://vuejs.org/guide/essentials/event-handling.html#key-modifiers</t>
+  </si>
+  <si>
+    <t>.enter</t>
+  </si>
+  <si>
+    <t>.tab</t>
+  </si>
+  <si>
+    <t>.esc</t>
+  </si>
+  <si>
+    <t>.space</t>
+  </si>
+  <si>
+    <t>.up</t>
+  </si>
+  <si>
+    <t>.down</t>
+  </si>
+  <si>
+    <t>.left</t>
+  </si>
+  <si>
+    <t>.right</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;input @keyup.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>page-down</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>="onPageDown" /&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;input @keyup</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.alt.enter</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>="clear" /&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>Модификаторы клавиш можно цеплять друг за друга</t>
+  </si>
+  <si>
+    <t>любые клавиши</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Возможно использовать любые клавишы</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+пропись названия клавишы должна быть в kebab case</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Исключения</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+.ctrl
+.alt
+.shift
+.meta</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>`@keyup.ctrl</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Модификаторы вроде .ctrl не отслеживают отпускание самой клавиши Ctrl, а проверяют:
+Была ли клавиша Ctrl нажата (удерживалась) в момент отпускания другой клавиши?
+Вы удерживаете Ctrl, затем нажимаете и отпускаете, например, S.
+→ Событие keyup произойдёт на клавише S, и при этом Ctrl всё ещё нажат.
+→ @keyup.ctrl сработает.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Исключения</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+.exact</t>
+    </r>
+  </si>
+  <si>
+    <t>Сработает, даже если (другие системные клавиши) Alt или Shift нажаты
+Сработает, только если Ctrl нажат
+Сработает, если системные клавиши не нажаты</t>
+  </si>
+  <si>
+    <t>.middle</t>
+  </si>
+  <si>
+    <t>(captures both "Delete" and "Backspace" keys)</t>
+  </si>
+  <si>
+    <t>.delete</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;input type=text" 
+v-bind:placeholder="placeholderString"
+v-bind:v-value="inputValue"
+v-on:input="inputChangeHandler(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>$event</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">)"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>v-on:keypress.enter="inputKeyPress"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+/&gt;
+…</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Важно - удобно! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Необязательно передавать параметром $event в метод, чтобы его затем получить в коде js</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&lt;button </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@click.ctrl</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>="onClick(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>$event</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">)"&gt;A&lt;/button&gt;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>$event.key</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - название нажатой кнпоки
+&lt;button </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@click.ctrl.exact</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">="onCtrlClick"&gt;A&lt;/button&gt;
+&lt;button </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@click.exact</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>="onClick"&gt;A&lt;/button&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Важно - удобно! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Необязательно передавать параметром </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>$event</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> в метод, чтобы его затем получить в коде js</t>
+    </r>
+  </si>
+  <si>
+    <t>Вызов нескольких функций/методов</t>
+  </si>
+  <si>
+    <t>chaining keys/buttons</t>
+  </si>
+  <si>
+    <t>chaining events</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Важно! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Используется по умолчанию для всех событий @click</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - по умолчанию специально он не указывается</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>`@click.right.prevent="</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>remove(i), log(item)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>`@click.right.prevent="</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{remove(i); log(item)}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <t>Возможность вызова нескольких методов для одного события</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">index.html
+&lt;div </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>id="app"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">&gt;  
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;h1&gt;&lt;/h1&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+&lt;/div&gt; указываем селектор id = app</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">app.js
+Vue.createApp({
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>//настройки приложения</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+}).mount(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'#app'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Достаточно начать писать html разметку</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">app.js
+Vue.createApp({
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> template: `
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  &lt;div&gt; class="card center"&gt;
+    &lt;h1&gt;{{ title }}&lt;/h1&gt;
+    &lt;button class="btn" @click="title = 'Изменили!'"&gt;Изменить&lt;/button&gt;
+   &lt;/div&gt;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>`</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+}).mount(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'#app'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">index.html
+&lt;div </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>id="app"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt;  
+&lt;/div&gt; указываем селектор id = app</t>
+    </r>
+  </si>
+  <si>
+    <t>Достаточно инициировать свойство template</t>
+  </si>
+  <si>
+    <t>Virtial DOM - то, что является основой vue.
+Все фреймворки решают одну проблему - оптимизацию общения javascript и dom дерева</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -4815,6 +5618,14 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -4895,10 +5706,10 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -4909,20 +5720,20 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -4931,71 +5742,80 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="8" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="49" fontId="5" fillId="9" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="9" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="10" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="11" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="2" applyFill="1"/>
-    <xf numFmtId="49" fontId="2" fillId="9" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="9" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="10" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="11" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2" xfId="1" xr:uid="{141A142D-D8A7-43F9-B8D2-54AA311FA1CB}"/>
     <cellStyle name="Обычный 2 2" xfId="2" xr:uid="{6AED7C1E-16D4-4B27-9CDE-4556C8555CBE}"/>
   </cellStyles>
@@ -5327,44 +6147,44 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:V71"/>
+  <dimension ref="A2:V97"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:D21"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="A8:B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="36" style="1" customWidth="1"/>
-    <col min="2" max="2" width="50.54296875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="81.08984375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="56.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.36328125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="43.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="55.08984375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="67.90625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="64.453125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="7.90625" style="7" customWidth="1"/>
-    <col min="11" max="11" width="39.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="48.90625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="72.54296875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="43.90625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="7.90625" style="7" customWidth="1"/>
-    <col min="16" max="16" width="56.90625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="46.6328125" style="2" customWidth="1"/>
-    <col min="18" max="18" width="62.90625" style="2" customWidth="1"/>
-    <col min="19" max="19" width="49.08984375" style="1" customWidth="1"/>
-    <col min="20" max="20" width="8.6328125" style="8"/>
-    <col min="21" max="21" width="67.6328125" style="2" customWidth="1"/>
-    <col min="22" max="22" width="68.453125" style="1" customWidth="1"/>
-    <col min="23" max="24" width="59.453125" style="1" customWidth="1"/>
-    <col min="25" max="25" width="59.54296875" style="1" customWidth="1"/>
-    <col min="26" max="26" width="99.453125" style="1" customWidth="1"/>
-    <col min="27" max="27" width="41.36328125" style="1" customWidth="1"/>
-    <col min="28" max="16384" width="8.6328125" style="1"/>
+    <col min="2" max="2" width="50.5546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="81.109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="56.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.33203125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="43.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="67.88671875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="64.44140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="7.88671875" style="7" customWidth="1"/>
+    <col min="11" max="11" width="39.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="48.88671875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="72.5546875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="43.88671875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="7.88671875" style="7" customWidth="1"/>
+    <col min="16" max="16" width="56.88671875" style="2" customWidth="1"/>
+    <col min="17" max="17" width="46.6640625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="62.88671875" style="2" customWidth="1"/>
+    <col min="19" max="19" width="49.109375" style="1" customWidth="1"/>
+    <col min="20" max="20" width="8.6640625" style="8"/>
+    <col min="21" max="21" width="67.6640625" style="2" customWidth="1"/>
+    <col min="22" max="22" width="68.44140625" style="1" customWidth="1"/>
+    <col min="23" max="24" width="59.44140625" style="1" customWidth="1"/>
+    <col min="25" max="25" width="59.5546875" style="1" customWidth="1"/>
+    <col min="26" max="26" width="99.44140625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="41.33203125" style="1" customWidth="1"/>
+    <col min="28" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="5"/>
       <c r="C2" s="6"/>
@@ -5383,7 +6203,7 @@
       <c r="S2" s="5"/>
       <c r="U2" s="5"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -5397,12 +6217,12 @@
       <c r="U3" s="1"/>
       <c r="V3" s="2"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="116" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -5414,557 +6234,961 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="58" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B7" s="13" t="s">
+    <row r="8" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C8" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" ht="58" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:22" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:22" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" ht="130.5" x14ac:dyDescent="0.35">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B11" s="13"/>
       <c r="C11" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="15" t="s">
-        <v>161</v>
-      </c>
       <c r="B12" s="15" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
     </row>
-    <row r="14" spans="1:22" ht="58" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" ht="116" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:22" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="B15" s="13" t="s">
-        <v>108</v>
-      </c>
       <c r="C15" s="13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" ht="72.5" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="13" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B17" s="12"/>
       <c r="C17" s="9"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="32" t="s">
-        <v>204</v>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="30" t="s">
+        <v>202</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="9"/>
     </row>
-    <row r="19" spans="1:4" ht="87" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="33" t="s">
-        <v>205</v>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="31" t="s">
+        <v>203</v>
       </c>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
     </row>
-    <row r="21" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="15"/>
-      <c r="C21" s="31" t="s">
-        <v>206</v>
+      <c r="C21" s="29" t="s">
+        <v>204</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B22" s="12"/>
       <c r="C22" s="9"/>
     </row>
-    <row r="23" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="130.5" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
       <c r="B24" s="12"/>
       <c r="C24" s="13" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C25" s="13"/>
     </row>
-    <row r="26" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="B27" s="13"/>
       <c r="C27" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="216" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="B28" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" s="15" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="217.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B28" s="13" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="10" t="s">
         <v>81</v>
-      </c>
-      <c r="C28" s="15" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="10" t="s">
-        <v>83</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="9"/>
     </row>
-    <row r="30" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B30" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="203" x14ac:dyDescent="0.35">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="201.6" x14ac:dyDescent="0.3">
       <c r="B31" s="12"/>
       <c r="C31" s="13" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B32" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C32" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="130.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="33" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B33" s="13"/>
       <c r="C33" s="13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="174" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
       <c r="B34" s="12"/>
       <c r="C34" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B35" s="12"/>
       <c r="C35" s="13"/>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="203" x14ac:dyDescent="0.35">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="201.6" x14ac:dyDescent="0.3">
       <c r="B37" s="12"/>
       <c r="C37" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="C38" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B38" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>113</v>
-      </c>
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B39" s="12"/>
       <c r="C39" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="87" x14ac:dyDescent="0.35">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B40" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C40" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="C40" s="13" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="17" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B41" s="13"/>
       <c r="C41" s="13"/>
       <c r="D41" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="B42" s="15" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" ht="188.5" x14ac:dyDescent="0.35">
-      <c r="B42" s="15" t="s">
+      <c r="C42" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="D42" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="C42" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="D42" s="15" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="10" t="s">
         <v>15</v>
       </c>
       <c r="B43" s="13"/>
       <c r="C43" s="13"/>
       <c r="D43" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="216" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B44" s="32" t="s">
+        <v>255</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="D44" s="15" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="216" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" ht="217.5" x14ac:dyDescent="0.35">
-      <c r="A44" s="1" t="s">
+      <c r="B45" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="C45" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="B44" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="C44" s="15" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="217.5" x14ac:dyDescent="0.35">
-      <c r="A45" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B45" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="C45" s="15" t="s">
+      <c r="D45" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="D45" s="15" t="s">
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A47" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="B47" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B48" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="C48" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C49" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A50" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B50" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="C50" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A51" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C51" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A52" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C52" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="15" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B46" s="15"/>
-      <c r="C46" s="15"/>
-      <c r="D46" s="15"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B47" s="15"/>
-      <c r="C47" s="15"/>
-      <c r="D47" s="15"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B48" s="15"/>
-      <c r="C48" s="15"/>
-      <c r="D48" s="15"/>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B49" s="15"/>
-      <c r="C49" s="15"/>
-      <c r="D49" s="15"/>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B50" s="15"/>
-      <c r="C50" s="15"/>
-      <c r="D50" s="15"/>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B51" s="15"/>
-      <c r="C51" s="15"/>
-      <c r="D51" s="15"/>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B52" s="15"/>
-      <c r="C52" s="15"/>
-      <c r="D52" s="15"/>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B53" s="15"/>
-      <c r="C53" s="15"/>
+      <c r="B53" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C53" s="15" t="s">
+        <v>200</v>
+      </c>
       <c r="D53" s="15"/>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B54" s="15"/>
-      <c r="C54" s="15"/>
-      <c r="D54" s="15"/>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B55" s="15"/>
-      <c r="C55" s="15"/>
-      <c r="D55" s="15"/>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B56" s="15"/>
-      <c r="C56" s="15"/>
-      <c r="D56" s="15"/>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B57" s="15"/>
-      <c r="C57" s="15"/>
-      <c r="D57" s="15"/>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B58" s="15"/>
-      <c r="C58" s="15"/>
-      <c r="D58" s="15"/>
-    </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B59" s="15"/>
-      <c r="C59" s="15"/>
+    <row r="54" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A54" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C54" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="D54" s="15" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A55" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C55" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="D55" s="15" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A56" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B56" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="C56" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A57" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B57" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="C57" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C58" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A59" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B59" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="C59" s="15" t="s">
+        <v>188</v>
+      </c>
       <c r="D59" s="15"/>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="10" t="s">
+        <v>194</v>
+      </c>
       <c r="B60" s="15"/>
       <c r="C60" s="15"/>
       <c r="D60" s="15"/>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B61" s="15"/>
-      <c r="C61" s="15"/>
+    <row r="61" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C61" s="15" t="s">
+        <v>195</v>
+      </c>
       <c r="D61" s="15"/>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B62" s="15"/>
-      <c r="C62" s="15"/>
+    <row r="62" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C62" s="29" t="s">
+        <v>196</v>
+      </c>
       <c r="D62" s="15"/>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B63" s="15"/>
-      <c r="C63" s="15"/>
+    <row r="63" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C63" s="15" t="s">
+        <v>199</v>
+      </c>
       <c r="D63" s="15"/>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="10" t="s">
+        <v>206</v>
+      </c>
       <c r="B64" s="15"/>
       <c r="C64" s="15"/>
-      <c r="D64" s="15"/>
-    </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B65" s="15"/>
-      <c r="C65" s="15"/>
-      <c r="D65" s="15"/>
-    </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B66" s="15"/>
-      <c r="C66" s="15"/>
-      <c r="D66" s="15"/>
-    </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="D64" s="15" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="30" t="s">
+        <v>202</v>
+      </c>
+      <c r="B65" s="12"/>
+      <c r="C65" s="9"/>
+    </row>
+    <row r="66" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A66" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B66" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="C66" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="31" t="s">
+        <v>203</v>
+      </c>
       <c r="B67" s="15"/>
       <c r="C67" s="15"/>
-      <c r="D67" s="15"/>
-    </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="68" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A68" s="2"/>
       <c r="B68" s="15"/>
-      <c r="C68" s="15"/>
-      <c r="D68" s="15"/>
-    </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C68" s="29" t="s">
+        <v>204</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="10" t="s">
+        <v>207</v>
+      </c>
       <c r="B69" s="15"/>
       <c r="C69" s="15"/>
-      <c r="D69" s="15"/>
-    </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B70" s="15"/>
-      <c r="C70" s="15"/>
-      <c r="D70" s="15"/>
-    </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B71" s="15"/>
-      <c r="C71" s="15"/>
-      <c r="D71" s="15"/>
+      <c r="D69" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A70" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C70" s="29" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A71" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C71" s="29" t="s">
+        <v>222</v>
+      </c>
+      <c r="D71" s="2"/>
+    </row>
+    <row r="72" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A72" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B72" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="C72" s="29" t="s">
+        <v>223</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A73" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C73" s="29" t="s">
+        <v>228</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A74" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C74" s="29" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A75" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C75" s="29" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C76" s="32" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C77" s="29" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C79" s="9"/>
+      <c r="D79" s="2"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C80" s="9"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C81" s="9"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C82" s="9"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C83" s="9"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C84" s="9"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C85" s="9"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A88" s="32" t="s">
+        <v>248</v>
+      </c>
+      <c r="B88" s="32"/>
+      <c r="C88" s="32" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A89" s="32" t="s">
+        <v>250</v>
+      </c>
+      <c r="B89" s="32" t="s">
+        <v>257</v>
+      </c>
+      <c r="C89" s="32" t="s">
+        <v>251</v>
+      </c>
+      <c r="D89" s="32" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A90" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B90" s="32" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A93" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B93" s="32" t="s">
+        <v>243</v>
+      </c>
+      <c r="C93" s="32" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C94" s="33" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" s="34" t="s">
+        <v>259</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C96" s="32" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>264</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="11" type="noConversion"/>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="10" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -5978,48 +7202,48 @@
   </sheetPr>
   <dimension ref="A1:V14"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="36" style="19" customWidth="1"/>
-    <col min="2" max="2" width="50.54296875" style="20" customWidth="1"/>
-    <col min="3" max="3" width="100.453125" style="20" customWidth="1"/>
-    <col min="4" max="4" width="56.453125" style="19" customWidth="1"/>
-    <col min="5" max="5" width="6.1796875" style="18" customWidth="1"/>
-    <col min="6" max="6" width="43.1796875" style="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="55.08984375" style="20" customWidth="1"/>
-    <col min="8" max="8" width="67.90625" style="19" customWidth="1"/>
-    <col min="9" max="9" width="64.36328125" style="19" customWidth="1"/>
-    <col min="10" max="10" width="7.81640625" style="18" customWidth="1"/>
-    <col min="11" max="11" width="39.1796875" style="19" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="48.90625" style="19" customWidth="1"/>
-    <col min="13" max="13" width="72.6328125" style="19" customWidth="1"/>
-    <col min="14" max="14" width="43.90625" style="19" customWidth="1"/>
-    <col min="15" max="15" width="7.81640625" style="18" customWidth="1"/>
-    <col min="16" max="16" width="56.81640625" style="20" customWidth="1"/>
-    <col min="17" max="17" width="46.81640625" style="20" customWidth="1"/>
-    <col min="18" max="18" width="62.90625" style="20" customWidth="1"/>
-    <col min="19" max="19" width="49.1796875" style="19" customWidth="1"/>
-    <col min="20" max="20" width="8.81640625" style="21"/>
-    <col min="21" max="21" width="67.81640625" style="20" customWidth="1"/>
-    <col min="22" max="22" width="68.36328125" style="19" customWidth="1"/>
-    <col min="23" max="24" width="59.36328125" style="19" customWidth="1"/>
-    <col min="25" max="25" width="59.6328125" style="19" customWidth="1"/>
-    <col min="26" max="26" width="99.453125" style="19" customWidth="1"/>
-    <col min="27" max="27" width="41.1796875" style="19" customWidth="1"/>
-    <col min="28" max="16384" width="8.81640625" style="19"/>
+    <col min="2" max="2" width="50.5546875" style="20" customWidth="1"/>
+    <col min="3" max="3" width="100.44140625" style="20" customWidth="1"/>
+    <col min="4" max="4" width="56.44140625" style="19" customWidth="1"/>
+    <col min="5" max="5" width="6.21875" style="18" customWidth="1"/>
+    <col min="6" max="6" width="43.21875" style="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.109375" style="20" customWidth="1"/>
+    <col min="8" max="8" width="67.88671875" style="19" customWidth="1"/>
+    <col min="9" max="9" width="64.33203125" style="19" customWidth="1"/>
+    <col min="10" max="10" width="7.77734375" style="18" customWidth="1"/>
+    <col min="11" max="11" width="39.21875" style="19" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="48.88671875" style="19" customWidth="1"/>
+    <col min="13" max="13" width="72.6640625" style="19" customWidth="1"/>
+    <col min="14" max="14" width="43.88671875" style="19" customWidth="1"/>
+    <col min="15" max="15" width="7.77734375" style="18" customWidth="1"/>
+    <col min="16" max="16" width="56.77734375" style="20" customWidth="1"/>
+    <col min="17" max="17" width="46.77734375" style="20" customWidth="1"/>
+    <col min="18" max="18" width="62.88671875" style="20" customWidth="1"/>
+    <col min="19" max="19" width="49.21875" style="19" customWidth="1"/>
+    <col min="20" max="20" width="8.77734375" style="21"/>
+    <col min="21" max="21" width="67.77734375" style="20" customWidth="1"/>
+    <col min="22" max="22" width="68.33203125" style="19" customWidth="1"/>
+    <col min="23" max="24" width="59.33203125" style="19" customWidth="1"/>
+    <col min="25" max="25" width="59.6640625" style="19" customWidth="1"/>
+    <col min="26" max="26" width="99.44140625" style="19" customWidth="1"/>
+    <col min="27" max="27" width="41.21875" style="19" customWidth="1"/>
+    <col min="28" max="16384" width="8.77734375" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A1" s="30"/>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A1" s="36"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="22"/>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -6038,131 +7262,131 @@
       <c r="S2" s="23"/>
       <c r="U2" s="23"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C3" s="24" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="P3" s="19"/>
       <c r="U3" s="19"/>
       <c r="V3" s="20"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="25" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="P4" s="19"/>
       <c r="U4" s="19"/>
       <c r="V4" s="20"/>
     </row>
-    <row r="5" spans="1:22" ht="58" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:22" ht="58" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="C6" s="15" t="s">
-        <v>152</v>
-      </c>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:22" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:22" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="25" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="15"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C11" s="35" t="s">
+        <v>153</v>
+      </c>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:22" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:22" ht="116" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:22" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:22" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>148</v>
-      </c>
       <c r="B13" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:22" ht="216" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C14" s="20" t="s">
         <v>142</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:22" ht="217.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="C14" s="20" t="s">
-        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -6179,43 +7403,43 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:V58"/>
+  <dimension ref="A2:V45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="36" style="1" customWidth="1"/>
-    <col min="2" max="2" width="62.90625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="81.08984375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="56.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.36328125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="43.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="55.08984375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="67.90625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="64.453125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="7.90625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="39.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="48.90625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="72.54296875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="43.90625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="7.90625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="56.90625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="46.6328125" style="2" customWidth="1"/>
-    <col min="18" max="18" width="62.90625" style="2" customWidth="1"/>
-    <col min="19" max="19" width="49.08984375" style="1" customWidth="1"/>
-    <col min="21" max="21" width="67.6328125" style="2" customWidth="1"/>
-    <col min="22" max="22" width="68.453125" style="1" customWidth="1"/>
-    <col min="23" max="24" width="59.453125" style="1" customWidth="1"/>
-    <col min="25" max="25" width="59.54296875" style="1" customWidth="1"/>
-    <col min="26" max="26" width="99.453125" style="1" customWidth="1"/>
-    <col min="27" max="27" width="41.36328125" style="1" customWidth="1"/>
-    <col min="28" max="16384" width="8.6328125" style="1"/>
+    <col min="2" max="2" width="62.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="56.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.33203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="43.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="67.88671875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="64.44140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="7.88671875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="39.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="48.88671875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="72.5546875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="43.88671875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="7.88671875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="56.88671875" style="2" customWidth="1"/>
+    <col min="17" max="17" width="46.6640625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="62.88671875" style="2" customWidth="1"/>
+    <col min="19" max="19" width="49.109375" style="1" customWidth="1"/>
+    <col min="21" max="21" width="67.6640625" style="2" customWidth="1"/>
+    <col min="22" max="22" width="68.44140625" style="1" customWidth="1"/>
+    <col min="23" max="24" width="59.44140625" style="1" customWidth="1"/>
+    <col min="25" max="25" width="59.5546875" style="1" customWidth="1"/>
+    <col min="26" max="26" width="99.44140625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="41.33203125" style="1" customWidth="1"/>
+    <col min="28" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B2" s="5"/>
       <c r="C2" s="6"/>
       <c r="G2" s="5"/>
@@ -6223,10 +7447,10 @@
       <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
       <c r="S2" s="5"/>
-      <c r="T2" s="29"/>
+      <c r="T2" s="28"/>
       <c r="U2" s="5"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C3" s="11" t="s">
         <v>1</v>
       </c>
@@ -6237,492 +7461,118 @@
       <c r="U3" s="1"/>
       <c r="V3" s="2"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
-        <v>7</v>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A4" s="34" t="s">
+        <v>31</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A5" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" ht="58" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>172</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>169</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B6" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>267</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>170</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>174</v>
+        <v>268</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="B8" s="32" t="s">
+        <v>270</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>269</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>176</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>177</v>
-      </c>
+        <v>271</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D10" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A11" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>202</v>
-      </c>
-      <c r="D11" s="15"/>
-    </row>
-    <row r="12" spans="1:22" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>179</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>187</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>186</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>192</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A16" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>188</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="D17" s="15"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="10" t="s">
-        <v>196</v>
-      </c>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-    </row>
-    <row r="19" spans="1:4" ht="58" x14ac:dyDescent="0.35">
-      <c r="C19" s="15" t="s">
-        <v>197</v>
-      </c>
-      <c r="D19" s="15"/>
-    </row>
-    <row r="20" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="C20" s="31" t="s">
-        <v>198</v>
-      </c>
-      <c r="D20" s="15"/>
-    </row>
-    <row r="21" spans="1:4" ht="87" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>201</v>
-      </c>
-      <c r="D21" s="15"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" s="32" t="s">
-        <v>204</v>
-      </c>
-      <c r="B23" s="12"/>
-      <c r="C23" s="9"/>
-    </row>
-    <row r="24" spans="1:4" ht="87" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>195</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" s="33" t="s">
-        <v>205</v>
-      </c>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-    </row>
-    <row r="26" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="2"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="31" t="s">
-        <v>206</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="10" t="s">
-        <v>209</v>
-      </c>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-    </row>
-    <row r="28" spans="1:4" ht="87" x14ac:dyDescent="0.35">
-      <c r="A28" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="C28" s="31" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="87" x14ac:dyDescent="0.35">
-      <c r="A29" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="C29" s="31" t="s">
-        <v>225</v>
-      </c>
-      <c r="D29" s="2"/>
-    </row>
-    <row r="30" spans="1:4" ht="87" x14ac:dyDescent="0.35">
-      <c r="A30" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="B30" s="31" t="s">
-        <v>228</v>
-      </c>
-      <c r="C30" s="31" t="s">
-        <v>226</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="116" x14ac:dyDescent="0.35">
-      <c r="A31" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="C31" s="31" t="s">
-        <v>231</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="C32" s="31" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="C33" s="31" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="87" x14ac:dyDescent="0.35">
-      <c r="A34" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="C34" s="31" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="58" x14ac:dyDescent="0.35">
-      <c r="A35" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="C35" s="31" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C37" s="9"/>
-      <c r="D37" s="2"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C38" s="9"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C39" s="9"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C40" s="9"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C41" s="9"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C42" s="9"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C43" s="9"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C47" s="27"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B48" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B49" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B50" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C38" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="C51" s="28" t="s">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B39" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D39" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B52" s="2" t="s">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B40" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="D40" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B53" s="2" t="s">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B41" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D41" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B54" s="2" t="s">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B42" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="D42" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B55" s="2" t="s">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B43" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="D43" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B56" s="2" t="s">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B44" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B57" s="2" t="s">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B45" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="D45" s="1" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B58" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>